<commit_message>
Added controller for send deals and top searches
</commit_message>
<xml_diff>
--- a/src/main/resources/menBoohooCoat.xlsx
+++ b/src/main/resources/menBoohooCoat.xlsx
@@ -170,6 +170,21 @@
     <t>men_boohoo_coat_10</t>
   </si>
   <si>
+    <t>https://media.boohoo.com/i/boohoo/bmm65763_navy_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>SKINNY FIT PINSTRIPE DOUBLE BREASTED SUIT</t>
+  </si>
+  <si>
+    <t>$40.00</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/skinny-fit-pinstripe-double-breasted-suit/MAN03215.html</t>
+  </si>
+  <si>
+    <t>men_boohoo_coat_11</t>
+  </si>
+  <si>
     <t>https://media.boohoo.com/i/boohoo/mzz13957_black_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
   </si>
   <si>
@@ -177,21 +192,6 @@
   </si>
   <si>
     <t>https://ca.boohoo.com/single-breasted-wool-mix-overcoat/MZZ13957.html</t>
-  </si>
-  <si>
-    <t>men_boohoo_coat_11</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/bmm65763_navy_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>SKINNY FIT PINSTRIPE DOUBLE BREASTED SUIT</t>
-  </si>
-  <si>
-    <t>$40.00</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/skinny-fit-pinstripe-double-breasted-suit/MAN03215.html</t>
   </si>
   <si>
     <t>men_boohoo_coat_12</t>
@@ -810,27 +810,27 @@
         <v>53</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F12" t="s" s="0">
         <v>59</v>
@@ -1010,7 +1010,7 @@
         <v>96</v>
       </c>
       <c r="E21" t="s" s="0">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F21" t="s" s="0">
         <v>97</v>

</xml_diff>